<commit_message>
Actualizo word y excel al momento
</commit_message>
<xml_diff>
--- a/Rubrica Obligatorio I DDA 2023.xlsx
+++ b/Rubrica Obligatorio I DDA 2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casa\Desktop\Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689E01B1-185C-4F94-B87F-25900E18763D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C1B08B-DE0C-4F2E-9BEE-A0796BF5233F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8A4943E7-259F-4590-A589-953D5FAC8EF1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Concepto</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>si</t>
+  </si>
+  <si>
+    <t>PENDIENTE PEGAR EL WORD</t>
   </si>
 </sst>
 </file>
@@ -595,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6826F6-BD4D-4236-BEDA-818E145B061B}">
-  <dimension ref="B1:C28"/>
+  <dimension ref="B1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +611,7 @@
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
@@ -616,13 +619,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
@@ -630,7 +633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
@@ -638,7 +641,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -646,13 +649,16 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
@@ -660,13 +666,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
@@ -674,13 +680,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
@@ -688,7 +694,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
@@ -696,7 +702,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -704,19 +710,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>17</v>
       </c>
@@ -726,7 +732,9 @@
       <c r="B17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
@@ -744,13 +752,17 @@
       <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="21" spans="2:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">

</xml_diff>